<commit_message>
new videos and better data
</commit_message>
<xml_diff>
--- a/data/rom.xlsx
+++ b/data/rom.xlsx
@@ -568,7 +568,7 @@
         <v>108.079044</v>
       </c>
       <c r="D2">
-        <v>113.135925</v>
+        <v>112.501404</v>
       </c>
       <c r="E2">
         <v>10.313354</v>
@@ -592,7 +592,7 @@
         <v>50.424469</v>
       </c>
       <c r="L2">
-        <v>8.104757</v>
+        <v>7.947767</v>
       </c>
       <c r="M2">
         <v>26.591285</v>
@@ -610,7 +610,7 @@
         <v>22.872435</v>
       </c>
       <c r="R2">
-        <v>31.944023</v>
+        <v>31.931187</v>
       </c>
       <c r="S2">
         <v>28.505802</v>
@@ -628,13 +628,13 @@
         <v>24.511876</v>
       </c>
       <c r="X2">
-        <v>103.074658</v>
+        <v>102.775753</v>
       </c>
       <c r="Y2">
         <v>12.572627</v>
       </c>
       <c r="Z2">
-        <v>72.452866</v>
+        <v>72.080811</v>
       </c>
       <c r="AA2">
         <v>12.515446</v>
@@ -643,7 +643,7 @@
         <v>139.32534</v>
       </c>
       <c r="AC2">
-        <v>51.409497</v>
+        <v>50.728452</v>
       </c>
       <c r="AD2">
         <v>47.936181</v>
@@ -818,7 +818,7 @@
         <v>29.243469</v>
       </c>
       <c r="X4">
-        <v>118.151722</v>
+        <v>118.145268</v>
       </c>
       <c r="Y4">
         <v>15.319778</v>
@@ -833,7 +833,7 @@
         <v>124.572948</v>
       </c>
       <c r="AC4">
-        <v>47.650786</v>
+        <v>47.621745</v>
       </c>
       <c r="AD4">
         <v>43.670429</v>
@@ -895,7 +895,7 @@
         <v>45.354683</v>
       </c>
       <c r="R5">
-        <v>43.385075</v>
+        <v>43.050717</v>
       </c>
       <c r="S5">
         <v>95.351772</v>
@@ -1037,94 +1037,94 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>78.937771</v>
+        <v>80.943821</v>
       </c>
       <c r="C7">
-        <v>136.394638</v>
+        <v>134.507798</v>
       </c>
       <c r="D7">
-        <v>132.089981</v>
+        <v>145.166512</v>
       </c>
       <c r="E7">
-        <v>164.219826</v>
+        <v>121.602272</v>
       </c>
       <c r="F7">
-        <v>112.755482</v>
+        <v>83.531475</v>
       </c>
       <c r="G7">
-        <v>26.40723</v>
+        <v>30.315319</v>
       </c>
       <c r="H7">
-        <v>22.808686</v>
+        <v>37.209151</v>
       </c>
       <c r="I7">
-        <v>25.611588</v>
+        <v>36.880951</v>
       </c>
       <c r="J7">
-        <v>52.269825</v>
+        <v>64.403607</v>
       </c>
       <c r="K7">
-        <v>43.305508</v>
+        <v>55.711391</v>
       </c>
       <c r="L7">
-        <v>43.359755</v>
+        <v>15.498488</v>
       </c>
       <c r="M7">
-        <v>34.48169</v>
+        <v>32.673904</v>
       </c>
       <c r="N7">
-        <v>83.033257</v>
+        <v>73.142105</v>
       </c>
       <c r="O7">
-        <v>73.846096</v>
+        <v>68.236695</v>
       </c>
       <c r="P7">
-        <v>56.643905</v>
+        <v>28.833284</v>
       </c>
       <c r="Q7">
-        <v>43.54307</v>
+        <v>28.814277</v>
       </c>
       <c r="R7">
-        <v>59.987545</v>
+        <v>44.043698</v>
       </c>
       <c r="S7">
-        <v>30.030495</v>
+        <v>89.722458</v>
       </c>
       <c r="T7">
-        <v>52.269825</v>
+        <v>64.403607</v>
       </c>
       <c r="U7">
-        <v>43.305508</v>
+        <v>55.711391</v>
       </c>
       <c r="V7">
-        <v>35.257138</v>
+        <v>41.598244</v>
       </c>
       <c r="W7">
-        <v>33.260284</v>
+        <v>24.20197</v>
       </c>
       <c r="X7">
-        <v>154.719683</v>
+        <v>145.872508</v>
       </c>
       <c r="Y7">
-        <v>179.091947</v>
+        <v>132.509443</v>
       </c>
       <c r="Z7">
-        <v>98.405285</v>
+        <v>71.147936</v>
       </c>
       <c r="AA7">
-        <v>94.1893</v>
+        <v>22.222866</v>
       </c>
       <c r="AB7">
-        <v>95.480473</v>
+        <v>152.690972</v>
       </c>
       <c r="AC7">
-        <v>144.881149</v>
+        <v>116.703219</v>
       </c>
       <c r="AD7">
-        <v>52.269825</v>
+        <v>64.403607</v>
       </c>
       <c r="AE7">
-        <v>43.305508</v>
+        <v>55.711391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>